<commit_message>
Fixed for MI methods, changed documentation to HTML
</commit_message>
<xml_diff>
--- a/Results/tabn209_21_SASS_populated.xlsx
+++ b/Results/tabn209_21_SASS_populated.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="674" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="674" uniqueCount="187">
   <si>
     <t>[Standard errors appear in parentheses]</t>
   </si>
@@ -236,22 +236,7 @@
     <t>85</t>
   </si>
   <si>
-    <t>(18.3)</t>
-  </si>
-  <si>
-    <t>(14.4)</t>
-  </si>
-  <si>
-    <t>(15.0)</t>
-  </si>
-  <si>
-    <t>(0.3)</t>
-  </si>
-  <si>
-    <t>(0.5)</t>
-  </si>
-  <si>
-    <t>(0.4)</t>
+    <t>†</t>
   </si>
   <si>
     <t/>
@@ -269,18 +254,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>(5.9)</t>
-  </si>
-  <si>
-    <t>(5.0)</t>
-  </si>
-  <si>
-    <t>(3.5)</t>
-  </si>
-  <si>
-    <t>(0.2)</t>
-  </si>
-  <si>
     <t>149</t>
   </si>
   <si>
@@ -296,15 +269,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>(6.2)</t>
-  </si>
-  <si>
-    <t>(5.2)</t>
-  </si>
-  <si>
-    <t>(4.0)</t>
-  </si>
-  <si>
     <t>42</t>
   </si>
   <si>
@@ -320,18 +284,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>(2.4)</t>
-  </si>
-  <si>
-    <t>(2.1)</t>
-  </si>
-  <si>
-    <t>(1.1)</t>
-  </si>
-  <si>
-    <t>(0.1)</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
@@ -341,15 +293,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>(1.8)</t>
-  </si>
-  <si>
-    <t>(1.5)</t>
-  </si>
-  <si>
-    <t>(0.8)</t>
-  </si>
-  <si>
     <t>459</t>
   </si>
   <si>
@@ -359,15 +302,6 @@
     <t>216</t>
   </si>
   <si>
-    <t>(8.7)</t>
-  </si>
-  <si>
-    <t>(7.5)</t>
-  </si>
-  <si>
-    <t>(4.8)</t>
-  </si>
-  <si>
     <t>596</t>
   </si>
   <si>
@@ -383,15 +317,6 @@
     <t>21</t>
   </si>
   <si>
-    <t>(9.8)</t>
-  </si>
-  <si>
-    <t>(7.0)</t>
-  </si>
-  <si>
-    <t>(5.7)</t>
-  </si>
-  <si>
     <t>863</t>
   </si>
   <si>
@@ -410,18 +335,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>(11.3)</t>
-  </si>
-  <si>
-    <t>(9.4)</t>
-  </si>
-  <si>
-    <t>(6.9)</t>
-  </si>
-  <si>
-    <t>(0.6)</t>
-  </si>
-  <si>
     <t>796</t>
   </si>
   <si>
@@ -437,30 +350,15 @@
     <t>28</t>
   </si>
   <si>
-    <t>(13.4)</t>
-  </si>
-  <si>
-    <t>(10.4)</t>
-  </si>
-  <si>
-    <t>(8.0)</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
-    <t>‡</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>†</t>
-  </si>
-  <si>
     <t>1,432</t>
   </si>
   <si>
@@ -479,18 +377,6 @@
     <t>50</t>
   </si>
   <si>
-    <t>(16.8)</t>
-  </si>
-  <si>
-    <t>(14.1)</t>
-  </si>
-  <si>
-    <t>(9.7)</t>
-  </si>
-  <si>
-    <t>(0.7)</t>
-  </si>
-  <si>
     <t>1,174</t>
   </si>
   <si>
@@ -509,27 +395,12 @@
     <t>46</t>
   </si>
   <si>
-    <t>(13.9)</t>
-  </si>
-  <si>
-    <t>(10.8)</t>
-  </si>
-  <si>
-    <t>(10.5)</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>(1.7)</t>
-  </si>
-  <si>
-    <t>(1.2)</t>
-  </si>
-  <si>
     <t>83</t>
   </si>
   <si>
@@ -539,15 +410,6 @@
     <t>39</t>
   </si>
   <si>
-    <t>(3.7)</t>
-  </si>
-  <si>
-    <t>(3.2)</t>
-  </si>
-  <si>
-    <t>(1.9)</t>
-  </si>
-  <si>
     <t>291</t>
   </si>
   <si>
@@ -557,15 +419,6 @@
     <t>139</t>
   </si>
   <si>
-    <t>(7.4)</t>
-  </si>
-  <si>
-    <t>(6.1)</t>
-  </si>
-  <si>
-    <t>(4.4)</t>
-  </si>
-  <si>
     <t>770</t>
   </si>
   <si>
@@ -575,12 +428,6 @@
     <t>356</t>
   </si>
   <si>
-    <t>(11.9)</t>
-  </si>
-  <si>
-    <t>(7.3)</t>
-  </si>
-  <si>
     <t>779</t>
   </si>
   <si>
@@ -596,15 +443,6 @@
     <t>27</t>
   </si>
   <si>
-    <t>(10.3)</t>
-  </si>
-  <si>
-    <t>(8.3)</t>
-  </si>
-  <si>
-    <t>(6.6)</t>
-  </si>
-  <si>
     <t>875</t>
   </si>
   <si>
@@ -617,12 +455,6 @@
     <t>34</t>
   </si>
   <si>
-    <t>(12.9)</t>
-  </si>
-  <si>
-    <t>(8.2)</t>
-  </si>
-  <si>
     <t>2,358</t>
   </si>
   <si>
@@ -641,48 +473,24 @@
     <t>86</t>
   </si>
   <si>
-    <t>(20.0)</t>
-  </si>
-  <si>
-    <t>(15.2)</t>
-  </si>
-  <si>
-    <t>(14.3)</t>
-  </si>
-  <si>
     <t>161</t>
   </si>
   <si>
     <t>75</t>
   </si>
   <si>
-    <t>(5.4)</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
-    <t>(2.0)</t>
-  </si>
-  <si>
-    <t>(1.0)</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>(1.4)</t>
-  </si>
-  <si>
     <t>62</t>
   </si>
   <si>
-    <t>(3.6)</t>
-  </si>
-  <si>
     <t>720</t>
   </si>
   <si>
@@ -692,12 +500,6 @@
     <t>323</t>
   </si>
   <si>
-    <t>(17.2)</t>
-  </si>
-  <si>
-    <t>(13.5)</t>
-  </si>
-  <si>
     <t>1,359</t>
   </si>
   <si>
@@ -707,12 +509,6 @@
     <t>633</t>
   </si>
   <si>
-    <t>(17.9)</t>
-  </si>
-  <si>
-    <t>(0.9)</t>
-  </si>
-  <si>
     <t>635</t>
   </si>
   <si>
@@ -722,15 +518,6 @@
     <t>313</t>
   </si>
   <si>
-    <t>(11.2)</t>
-  </si>
-  <si>
-    <t>(9.6)</t>
-  </si>
-  <si>
-    <t>(6.0)</t>
-  </si>
-  <si>
     <t>223</t>
   </si>
   <si>
@@ -743,9 +530,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>(6.7)</t>
-  </si>
-  <si>
     <t>671</t>
   </si>
   <si>
@@ -758,12 +542,6 @@
     <t>18</t>
   </si>
   <si>
-    <t>(16.6)</t>
-  </si>
-  <si>
-    <t>(11.8)</t>
-  </si>
-  <si>
     <t>891</t>
   </si>
   <si>
@@ -773,9 +551,6 @@
     <t>401</t>
   </si>
   <si>
-    <t>(17.6)</t>
-  </si>
-  <si>
     <t>787</t>
   </si>
   <si>
@@ -791,24 +566,12 @@
     <t>19</t>
   </si>
   <si>
-    <t>(16.2)</t>
-  </si>
-  <si>
-    <t>(9.5)</t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
     <t>54</t>
   </si>
   <si>
-    <t>(7.9)</t>
-  </si>
-  <si>
-    <t>(5.8)</t>
-  </si>
-  <si>
     <t>2,714</t>
   </si>
   <si>
@@ -821,12 +584,6 @@
     <t>100</t>
   </si>
   <si>
-    <t>(22.1)</t>
-  </si>
-  <si>
-    <t>(16.7)</t>
-  </si>
-  <si>
     <t>680</t>
   </si>
   <si>
@@ -837,12 +594,6 @@
   </si>
   <si>
     <t>40</t>
-  </si>
-  <si>
-    <t>(10.0)</t>
-  </si>
-  <si>
-    <t>(5.5)</t>
   </si>
   <si>
     <t>2,034</t>
@@ -1670,58 +1421,58 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>254</v>
+        <v>175</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>258</v>
+        <v>63</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>255</v>
+        <v>176</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>259</v>
+        <v>63</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>256</v>
+        <v>177</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>257</v>
+        <v>178</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>257</v>
+        <v>178</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>257</v>
+        <v>178</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -1752,58 +1503,58 @@
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>260</v>
+        <v>179</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>264</v>
+        <v>63</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>261</v>
+        <v>180</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>265</v>
+        <v>63</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>262</v>
+        <v>181</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>191</v>
+        <v>63</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="O8" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P8" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>263</v>
+        <v>182</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S8" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9">
@@ -1811,58 +1562,58 @@
         <v>10</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>266</v>
+        <v>183</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>220</v>
+        <v>63</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>267</v>
+        <v>184</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>268</v>
+        <v>185</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>238</v>
+        <v>63</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>202</v>
+        <v>143</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P9" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>269</v>
+        <v>186</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
@@ -1896,7 +1647,7 @@
         <v>58</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>63</v>
@@ -1905,46 +1656,46 @@
         <v>59</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>60</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>61</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N11" s="21" t="s">
         <v>61</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q11" s="19" t="s">
         <v>62</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S11" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12">
@@ -1952,58 +1703,58 @@
         <v>12</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P12" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R12" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S12" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -2011,58 +1762,58 @@
         <v>13</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="O13" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P13" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R13" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S13" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" ht="30">
@@ -2070,58 +1821,58 @@
         <v>40</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="O14" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P14" s="22" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="R14" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" ht="30">
@@ -2129,58 +1880,58 @@
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="N15" s="21" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P15" s="22" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="R15" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S15" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16">
@@ -2211,58 +1962,58 @@
         <v>56</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="O17" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="R17" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S17" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18">
@@ -2270,58 +2021,58 @@
         <v>57</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P18" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="R18" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S18" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19">
@@ -2329,58 +2080,58 @@
         <v>15</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M19" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P19" s="22" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R19" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S19" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20">
@@ -2388,58 +2139,58 @@
         <v>41</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="O20" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P20" s="22" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R20" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S20" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
@@ -2470,58 +2221,58 @@
         <v>52</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="O22" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P22" s="22" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="Q22" s="19" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="R22" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S22" s="20" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23">
@@ -2529,58 +2280,58 @@
         <v>53</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P23" s="22" t="s">
-        <v>147</v>
+        <v>63</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="R23" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S23" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24">
@@ -2588,58 +2339,58 @@
         <v>49</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>154</v>
+        <v>63</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>155</v>
+        <v>63</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>156</v>
+        <v>63</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="O24" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P24" s="22" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="R24" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S24" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25">
@@ -2647,58 +2398,58 @@
         <v>51</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>160</v>
+        <v>63</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="O25" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P25" s="22" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="Q25" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="R25" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S25" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" ht="30">
@@ -2706,58 +2457,58 @@
         <v>50</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>164</v>
+        <v>63</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>165</v>
+        <v>63</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>166</v>
+        <v>63</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="N26" s="21" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P26" s="22" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="Q26" s="19" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="R26" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S26" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" ht="30">
@@ -2788,58 +2539,58 @@
         <v>16</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>171</v>
+        <v>63</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>172</v>
+        <v>63</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M28" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N28" s="21" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="O28" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P28" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="Q28" s="19" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="R28" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S28" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29">
@@ -2847,58 +2598,58 @@
         <v>17</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>177</v>
+        <v>63</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M29" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N29" s="21" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="O29" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P29" s="22" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="R29" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S29" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30">
@@ -2906,58 +2657,58 @@
         <v>18</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>184</v>
+        <v>63</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>185</v>
+        <v>63</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N30" s="21" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="O30" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P30" s="22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q30" s="19" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
       <c r="R30" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S30" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31">
@@ -2965,58 +2716,58 @@
         <v>19</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>186</v>
+        <v>132</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>187</v>
+        <v>133</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>188</v>
+        <v>134</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>191</v>
+        <v>63</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N31" s="21" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="O31" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P31" s="22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="R31" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S31" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" ht="26.25" customHeight="true">
@@ -3047,58 +2798,58 @@
         <v>20</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>198</v>
+        <v>63</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>200</v>
+        <v>63</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="L33" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M33" s="20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="N33" s="21" t="s">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="O33" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P33" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="Q33" s="19" t="s">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="R33" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S33" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34">
@@ -3106,58 +2857,58 @@
         <v>21</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>202</v>
+        <v>143</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>165</v>
+        <v>63</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="L34" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M34" s="20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="N34" s="21" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="O34" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P34" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q34" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="R34" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S34" s="20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" ht="26.25" customHeight="true">
@@ -3165,58 +2916,58 @@
         <v>22</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>204</v>
+        <v>144</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>205</v>
+        <v>63</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>206</v>
+        <v>63</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="L35" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M35" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="N35" s="21" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="O35" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P35" s="22" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="R35" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S35" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36">
@@ -3224,58 +2975,58 @@
         <v>23</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>207</v>
+        <v>145</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>209</v>
+        <v>63</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="L36" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M36" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="O36" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P36" s="22" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="Q36" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="R36" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S36" s="20" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37">
@@ -3283,58 +3034,58 @@
         <v>24</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>210</v>
+        <v>147</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>211</v>
+        <v>63</v>
       </c>
       <c r="K37" s="19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L37" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M37" s="20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="N37" s="21" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="O37" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P37" s="22" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="Q37" s="19" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="R37" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S37" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" ht="26.25" customHeight="true">
@@ -3365,58 +3116,58 @@
         <v>42</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>212</v>
+        <v>148</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>215</v>
+        <v>63</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>213</v>
+        <v>149</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>216</v>
+        <v>63</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
       <c r="L39" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M39" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
       <c r="O39" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P39" s="22" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="Q39" s="19" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="R39" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S39" s="20" t="s">
-        <v>147</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" ht="45">
@@ -3424,58 +3175,58 @@
         <v>43</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>217</v>
+        <v>151</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>220</v>
+        <v>63</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>218</v>
+        <v>152</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>219</v>
+        <v>153</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>154</v>
+        <v>63</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="L40" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M40" s="20" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="N40" s="21" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="O40" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P40" s="22" t="s">
-        <v>221</v>
+        <v>63</v>
       </c>
       <c r="Q40" s="19" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="R40" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S40" s="20" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" ht="30">
@@ -3483,58 +3234,58 @@
         <v>44</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>222</v>
+        <v>154</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>225</v>
+        <v>63</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>223</v>
+        <v>155</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>226</v>
+        <v>63</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>227</v>
+        <v>63</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="L41" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M41" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N41" s="21" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="O41" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P41" s="22" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="Q41" s="19" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="R41" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S41" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" ht="53" customHeight="true">
@@ -3565,58 +3316,58 @@
         <v>45</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>228</v>
+        <v>157</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>225</v>
+        <v>63</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>230</v>
+        <v>159</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>232</v>
+        <v>63</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="L43" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M43" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N43" s="21" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="O43" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P43" s="22" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="Q43" s="19" t="s">
-        <v>231</v>
+        <v>160</v>
       </c>
       <c r="R43" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S43" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44">
@@ -3624,58 +3375,58 @@
         <v>46</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>233</v>
+        <v>161</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>234</v>
+        <v>162</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>238</v>
+        <v>63</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>235</v>
+        <v>163</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>225</v>
+        <v>63</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="L44" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M44" s="20" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="N44" s="21" t="s">
-        <v>236</v>
+        <v>164</v>
       </c>
       <c r="O44" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P44" s="22" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="Q44" s="19" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="R44" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S44" s="20" t="s">
-        <v>147</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45">
@@ -3683,58 +3434,58 @@
         <v>47</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>242</v>
+        <v>63</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>240</v>
+        <v>166</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>241</v>
+        <v>167</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="L45" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>147</v>
+        <v>63</v>
       </c>
       <c r="N45" s="21" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="O45" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P45" s="22" t="s">
-        <v>206</v>
+        <v>63</v>
       </c>
       <c r="Q45" s="19" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="R45" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S45" s="20" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46">
@@ -3742,58 +3493,58 @@
         <v>48</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>243</v>
+        <v>168</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D46" s="16" t="s">
         <v>63</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>244</v>
+        <v>169</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>248</v>
+        <v>63</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>245</v>
+        <v>170</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>249</v>
+        <v>63</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="L46" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="N46" s="21" t="s">
-        <v>246</v>
+        <v>171</v>
       </c>
       <c r="O46" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P46" s="22" t="s">
-        <v>221</v>
+        <v>63</v>
       </c>
       <c r="Q46" s="19" t="s">
-        <v>247</v>
+        <v>172</v>
       </c>
       <c r="R46" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S46" s="20" t="s">
-        <v>147</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" ht="30">
@@ -3801,58 +3552,58 @@
         <v>25</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>250</v>
+        <v>173</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>252</v>
+        <v>63</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>251</v>
+        <v>174</v>
       </c>
       <c r="F47" s="27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J47" s="16" t="s">
-        <v>253</v>
+        <v>63</v>
       </c>
       <c r="K47" s="29" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L47" s="27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M47" s="30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N47" s="21" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="O47" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P47" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q47" s="29" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="R47" s="27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S47" s="30" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48">

</xml_diff>